<commit_message>
add markdown for academicpeak
</commit_message>
<xml_diff>
--- a/academicpeak/database.xlsx
+++ b/academicpeak/database.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hongzhe.site\academicpeak\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xieho\PycharmProjects\hongzhe.site\academicpeak\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FBB28A6-F7F5-407C-9A80-6802370A202E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F39FE2-0F00-4684-B878-4660A87A387B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="180" windowWidth="46200" windowHeight="5850" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -319,17 +319,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -369,7 +369,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -649,21 +649,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="38.875" customWidth="1"/>
-    <col min="3" max="3" width="16.875" customWidth="1"/>
-    <col min="4" max="4" width="15.625" customWidth="1"/>
-    <col min="5" max="5" width="11.375" customWidth="1"/>
-    <col min="6" max="6" width="81.75" customWidth="1"/>
-    <col min="7" max="7" width="94.375" customWidth="1"/>
+    <col min="2" max="2" width="38.88671875" customWidth="1"/>
+    <col min="3" max="3" width="16.88671875" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" customWidth="1"/>
+    <col min="5" max="5" width="11.44140625" customWidth="1"/>
+    <col min="6" max="6" width="81.6640625" customWidth="1"/>
+    <col min="7" max="7" width="94.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -686,7 +686,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -701,7 +701,7 @@
       </c>
       <c r="E2">
         <f ca="1">INT(RAND()*100000)</f>
-        <v>90171</v>
+        <v>98892</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -710,12 +710,12 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
+      <c r="B3" t="s">
+        <v>43</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
@@ -725,21 +725,21 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E25" ca="1" si="0">INT(RAND()*100000)</f>
-        <v>90216</v>
+        <v>2999</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>44</v>
       </c>
       <c r="G3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>16</v>
@@ -749,21 +749,21 @@
       </c>
       <c r="E4">
         <f t="shared" ca="1" si="0"/>
-        <v>9942</v>
+        <v>34924</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>43</v>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>16</v>
@@ -773,16 +773,16 @@
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>37461</v>
+        <v>30363</v>
       </c>
       <c r="F5" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
@@ -797,7 +797,7 @@
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>7597</v>
+        <v>90762</v>
       </c>
       <c r="F6" t="s">
         <v>38</v>
@@ -806,7 +806,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
@@ -821,7 +821,7 @@
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>28921</v>
+        <v>76857</v>
       </c>
       <c r="F7" t="s">
         <v>11</v>
@@ -830,7 +830,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
@@ -845,7 +845,7 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>72676</v>
+        <v>41576</v>
       </c>
       <c r="F8" t="s">
         <v>46</v>
@@ -854,7 +854,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
@@ -869,7 +869,7 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>65323</v>
+        <v>86226</v>
       </c>
       <c r="F9" t="s">
         <v>10</v>
@@ -878,7 +878,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
@@ -893,7 +893,7 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>9371</v>
+        <v>57350</v>
       </c>
       <c r="F10" t="s">
         <v>50</v>
@@ -902,7 +902,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
@@ -917,7 +917,7 @@
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>92673</v>
+        <v>95919</v>
       </c>
       <c r="F11" t="s">
         <v>55</v>
@@ -926,7 +926,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
@@ -941,7 +941,7 @@
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>94644</v>
+        <v>84664</v>
       </c>
       <c r="F12" t="s">
         <v>33</v>
@@ -950,7 +950,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>12</v>
       </c>
@@ -965,7 +965,7 @@
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>10609</v>
+        <v>54212</v>
       </c>
       <c r="F13" t="s">
         <v>34</v>
@@ -974,7 +974,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>13</v>
       </c>
@@ -989,7 +989,7 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>59137</v>
+        <v>24023</v>
       </c>
       <c r="F14" t="s">
         <v>35</v>
@@ -998,7 +998,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1013,7 +1013,7 @@
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>65920</v>
+        <v>40729</v>
       </c>
       <c r="F15" t="s">
         <v>58</v>
@@ -1022,7 +1022,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1037,7 +1037,7 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>64768</v>
+        <v>19854</v>
       </c>
       <c r="F16" t="s">
         <v>36</v>
@@ -1046,7 +1046,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1061,7 +1061,7 @@
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>48405</v>
+        <v>91926</v>
       </c>
       <c r="F17" t="s">
         <v>37</v>
@@ -1070,7 +1070,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1085,7 +1085,7 @@
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="0"/>
-        <v>82196</v>
+        <v>44903</v>
       </c>
       <c r="F18" t="s">
         <v>39</v>
@@ -1094,7 +1094,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1109,7 +1109,7 @@
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="0"/>
-        <v>12034</v>
+        <v>72848</v>
       </c>
       <c r="F19" t="s">
         <v>40</v>
@@ -1118,7 +1118,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="0"/>
-        <v>46938</v>
+        <v>65145</v>
       </c>
       <c r="F20" t="s">
         <v>53</v>
@@ -1142,7 +1142,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1157,7 +1157,7 @@
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="0"/>
-        <v>78353</v>
+        <v>25744</v>
       </c>
       <c r="F21" t="s">
         <v>59</v>
@@ -1166,7 +1166,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="0"/>
-        <v>63784</v>
+        <v>65998</v>
       </c>
       <c r="F22" t="s">
         <v>47</v>
@@ -1190,7 +1190,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1205,7 +1205,7 @@
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="0"/>
-        <v>32551</v>
+        <v>94472</v>
       </c>
       <c r="F23" t="s">
         <v>20</v>
@@ -1214,7 +1214,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1229,7 +1229,7 @@
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="0"/>
-        <v>58713</v>
+        <v>62513</v>
       </c>
       <c r="F24" t="s">
         <v>32</v>
@@ -1238,7 +1238,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1253,7 +1253,7 @@
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="0"/>
-        <v>51933</v>
+        <v>85590</v>
       </c>
       <c r="F25" t="s">
         <v>31</v>
@@ -1269,7 +1269,7 @@
     <hyperlink ref="B9" r:id="rId2" display="https://www.usnews.com/education/best-global-universities/harvard-university-166027" xr:uid="{7978A213-D431-46CF-8201-9BA0735B8A3F}"/>
     <hyperlink ref="B7" r:id="rId3" display="https://www.usnews.com/education/best-global-universities/university-of-california-berkeley-110635" xr:uid="{4D75220F-9B33-4F4D-8693-69911F9519C8}"/>
     <hyperlink ref="F7" r:id="rId4" xr:uid="{CDF58638-52C8-4B3B-AD1A-A2C6BA2650B4}"/>
-    <hyperlink ref="F4" r:id="rId5" xr:uid="{D6A8DE96-784D-4552-9293-D51126E14D21}"/>
+    <hyperlink ref="F5" r:id="rId5" xr:uid="{D6A8DE96-784D-4552-9293-D51126E14D21}"/>
     <hyperlink ref="F23" r:id="rId6" xr:uid="{D4ED1D55-E4AC-4C6B-85A0-E974BD65D69E}"/>
     <hyperlink ref="F25" r:id="rId7" xr:uid="{BC2E73A6-CC84-4897-A562-432D2F10BD7D}"/>
     <hyperlink ref="F24" r:id="rId8" xr:uid="{C011FDAA-A7A1-4B75-A45E-5CDE4F833888}"/>

</xml_diff>